<commit_message>
cambios menores,organizacion y limpieza de carpetas y rutas, en testeo y liberacion de aplicacion
</commit_message>
<xml_diff>
--- a/data/MF-64_plantilla.xlsx
+++ b/data/MF-64_plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_oneasg_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/mantto_feeder/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_FD60740C77BB531F1E02F60B334016B7677A8072" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A8992DA-3C1E-4102-8EC7-43585E2E73D2}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_A0FB244937561196E9F67CF6E4DD334938563519" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF958457-1D2A-4791-81F8-D91A121AE7EB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,14 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Checklist!$B$1:$E$33</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">BITÁCORA DE MANTENIMIENTO PROGRAMADO </t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+  <si>
+    <t xml:space="preserve">   BITÁCORA DE MANTENIMIENTO PROGRAMADO </t>
   </si>
   <si>
     <t xml:space="preserve"> "PARA FEEDERS"</t>
@@ -47,15 +36,24 @@
     <t>Fecha:</t>
   </si>
   <si>
+    <t>4_Jul_2023</t>
+  </si>
+  <si>
     <t>Tecnico:</t>
   </si>
   <si>
+    <t>Cristian Echevarria</t>
+  </si>
+  <si>
     <t>No. de ID:</t>
   </si>
   <si>
     <t>Color:</t>
   </si>
   <si>
+    <t>ROJO</t>
+  </si>
+  <si>
     <t>Área:                                 Actividad:</t>
   </si>
   <si>
@@ -74,6 +72,9 @@
     <t>Alcohol, Biral y llaves allen</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>lubricacion de valeros</t>
   </si>
   <si>
@@ -114,9 +115,6 @@
   </si>
   <si>
     <t>Alcohol, Biral, Daphne</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t xml:space="preserve"> desarmador plano, llaves allen </t>
@@ -225,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -271,6 +269,25 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto Black"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -286,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -435,9 +452,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -449,7 +464,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -459,7 +476,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -475,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -509,72 +552,53 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -584,105 +608,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BC8033-94CA-64F8-15E0-8F74939D36DC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2028825" y="590550"/>
-          <a:ext cx="1819275" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>28631</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114374</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1333500" cy="266700"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -975,7 +900,7 @@
   <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1005,41 +930,43 @@
       <c r="A3" s="4"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="33"/>
@@ -1066,13 +993,17 @@
       <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="41"/>
+      <c r="B12" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="42"/>
       <c r="E12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+        <v>4</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="42"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1082,15 +1013,19 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
+        <v>6</v>
+      </c>
+      <c r="B14" s="41">
+        <v>23760055</v>
+      </c>
+      <c r="C14" s="42"/>
       <c r="E14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="42"/>
       <c r="H14" s="5"/>
       <c r="K14" s="11"/>
     </row>
@@ -1101,17 +1036,17 @@
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H16" s="12"/>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E17" s="6"/>
       <c r="H17" s="12"/>
@@ -1119,76 +1054,76 @@
     </row>
     <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
         <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H24" s="5"/>
     </row>
@@ -1198,42 +1133,42 @@
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H29" s="5"/>
     </row>
@@ -1243,62 +1178,62 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H36" s="5"/>
     </row>
@@ -1308,66 +1243,66 @@
     </row>
     <row r="38" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H44" s="5"/>
     </row>
@@ -1391,7 +1326,7 @@
     </row>
     <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1412,221 +1347,221 @@
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="37"/>
+      <c r="A65" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="34"/>
     </row>
     <row r="66" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="35"/>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="37"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="34"/>
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="37"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="34"/>
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="35"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="37"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="34"/>
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="35"/>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="37"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="34"/>
     </row>
     <row r="70" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="35"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="37"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="34"/>
     </row>
     <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="35"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="37"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="34"/>
     </row>
     <row r="72" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="35"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="37"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="34"/>
     </row>
     <row r="73" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="35"/>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="37"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="34"/>
     </row>
     <row r="74" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="35"/>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="37"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="34"/>
     </row>
     <row r="75" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="35"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="37"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="33"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="34"/>
     </row>
     <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="35"/>
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="37"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="34"/>
     </row>
     <row r="77" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="35"/>
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="37"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="34"/>
     </row>
     <row r="78" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="35"/>
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="37"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="34"/>
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="35"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="36"/>
-      <c r="G79" s="36"/>
-      <c r="H79" s="37"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="33"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="34"/>
     </row>
     <row r="80" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="35"/>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="37"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="34"/>
     </row>
     <row r="81" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="35"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="37"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="34"/>
     </row>
     <row r="82" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="35"/>
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="36"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="37"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="34"/>
     </row>
     <row r="83" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="35"/>
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="37"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="34"/>
     </row>
     <row r="84" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="35"/>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="37"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="33"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="34"/>
     </row>
     <row r="85" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="35"/>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="37"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="34"/>
     </row>
     <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="38"/>
@@ -1651,18 +1586,15 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter xml:space="preserve">&amp;L&amp;7MF-64 Rev:05
-&amp;6&amp;Z&amp;F&amp;C&amp;7Retencion: 2 años
-_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.&amp;R&amp;7Relacionada con: 7.1-11 III 
-</oddFooter>
-    <evenFooter xml:space="preserve">&amp;L&amp;7MF-64 Rev:05
-&amp;6&amp;Z&amp;F&amp;C&amp;7Retencion: 2 años
-&amp;R&amp;7Relacionada con: 7.1-11 III 
-</evenFooter>
+    <oddFooter>&amp;L&amp;6 MF-64 Rev:05
+&amp;Z&amp;F&amp;C&amp;"Calibri"&amp;10 &amp;K0000FFRetencion: 2 años
+_x000D_# This data is internal to Brunswick._x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.&amp;R&amp;7 Relacionada con: 7.1-11 III</oddFooter>
+    <evenFooter>&amp;L&amp;6 MF-64 Rev:05
+&amp;Z&amp;F&amp;C&amp;7 Retencion: 2 años
+&amp;R&amp;7 Relacionada con: 7.1-11 III</evenFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1685,12 +1617,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="19"/>
@@ -1698,26 +1630,26 @@
     </row>
     <row r="4" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -1725,23 +1657,23 @@
     <row r="6" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>11</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="14"/>
@@ -1749,36 +1681,36 @@
     <row r="8" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="14"/>
@@ -1786,20 +1718,20 @@
     <row r="11" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19"/>
       <c r="C11" s="14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="14"/>
@@ -1807,10 +1739,10 @@
     <row r="13" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19"/>
       <c r="C13" s="14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="14"/>
@@ -1818,10 +1750,10 @@
     <row r="14" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19"/>
       <c r="C14" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="14"/>
@@ -1829,17 +1761,17 @@
     <row r="15" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="14"/>
@@ -1847,10 +1779,10 @@
     <row r="17" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="14"/>
@@ -1858,10 +1790,10 @@
     <row r="18" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="14"/>
@@ -1869,10 +1801,10 @@
     <row r="19" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
       <c r="C19" s="14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="14"/>
@@ -1880,10 +1812,10 @@
     <row r="20" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19"/>
       <c r="C20" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="14"/>
@@ -1891,29 +1823,29 @@
     <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
       <c r="C21" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E22" s="20"/>
     </row>
     <row r="23" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19"/>
       <c r="C23" s="14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="14"/>
@@ -1921,10 +1853,10 @@
     <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="19"/>
       <c r="C24" s="14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="14"/>
@@ -1932,20 +1864,20 @@
     <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="19"/>
       <c r="C25" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="14"/>
     </row>
     <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="14"/>
@@ -1953,7 +1885,7 @@
     <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="19"/>
       <c r="C27" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="14"/>
@@ -1961,10 +1893,10 @@
     <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="19"/>
       <c r="C28" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="14"/>
@@ -1972,10 +1904,10 @@
     <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="19"/>
       <c r="C29" s="14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="14"/>
@@ -1983,10 +1915,10 @@
     <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19"/>
       <c r="C30" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="14"/>
@@ -1994,7 +1926,7 @@
     <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="19"/>
       <c r="C31" s="14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="14"/>
@@ -2002,10 +1934,10 @@
     <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="19"/>
       <c r="C32" s="14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="14"/>
@@ -2013,10 +1945,10 @@
     <row r="33" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="24"/>
       <c r="C33" s="25" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E33" s="26"/>
     </row>
@@ -2028,11 +1960,10 @@
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;LMF-64 Rev:04
-&amp;Z&amp;F&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.&amp;RRELACIONADO CON: 7.1-11</oddFooter>
+&amp;Z&amp;F&amp;C&amp;"Calibri"&amp;10 &amp;K0000FF_x000D_# This data is internal to Brunswick._x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.&amp;RRELACIONADO CON: 7.1-11</oddFooter>
     <evenFooter>&amp;LMF-64 Rev:04
 &amp;Z&amp;F&amp;RRELACIONADO CON: 7.1-11</evenFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2046,7 +1977,7 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.</oddFooter>
+    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K0000FF_x000D_# This data is internal to Brunswick._x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lanzando proyecto a produccion,se agrego validacion de id de tecnico para poder generar reporte con su nombre..., de igual forma se estara buscando retroalimentacion por parte del departamento de feeder setup
</commit_message>
<xml_diff>
--- a/data/MF-64_plantilla.xlsx
+++ b/data/MF-64_plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_oneasg_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/mantto_feeder/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_A0FB244937561196E9F67CF6E4DD334938563519" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF958457-1D2A-4791-81F8-D91A121AE7EB}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_A0FB244937561196E9F67CF6E4DD334938563519" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BC09B8-3CE7-4FB4-8304-7DD0F7CFF5E3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -608,6 +608,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DFDB107-FE3E-185D-7D39-55DADA37332A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2114550" y="600075"/>
+          <a:ext cx="1819275" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -900,7 +955,7 @@
   <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+      <selection activeCell="O13" sqref="O13:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1595,6 +1650,7 @@
 &amp;Z&amp;F&amp;C&amp;7 Retencion: 2 años
 &amp;R&amp;7 Relacionada con: 7.1-11 III</evenFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cambios menores,reporte ya no pierde imagen al momento de manipular archivo,lanzada a produccion exitosamente
</commit_message>
<xml_diff>
--- a/data/MF-64_plantilla.xlsx
+++ b/data/MF-64_plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_oneasg_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/mantto_feeder/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_A0FB244937561196E9F67CF6E4DD334938563519" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BC09B8-3CE7-4FB4-8304-7DD0F7CFF5E3}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_A0FB244937561196E9F67CF6E4DD334938563519" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{446F01E0-31FF-4515-9643-7D0323ED4EAF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="1395" windowWidth="21255" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
   <si>
     <t xml:space="preserve">   BITÁCORA DE MANTENIMIENTO PROGRAMADO </t>
   </si>
@@ -36,22 +36,13 @@
     <t>Fecha:</t>
   </si>
   <si>
-    <t>4_Jul_2023</t>
-  </si>
-  <si>
     <t>Tecnico:</t>
   </si>
   <si>
-    <t>Cristian Echevarria</t>
-  </si>
-  <si>
     <t>No. de ID:</t>
   </si>
   <si>
     <t>Color:</t>
-  </si>
-  <si>
-    <t>ROJO</t>
   </si>
   <si>
     <t>Área:                                 Actividad:</t>
@@ -608,61 +599,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DFDB107-FE3E-185D-7D39-55DADA37332A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2114550" y="600075"/>
-          <a:ext cx="1819275" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -955,7 +891,7 @@
   <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:O14"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1048,16 +984,12 @@
       <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>3</v>
-      </c>
+      <c r="B12" s="43"/>
       <c r="C12" s="42"/>
       <c r="E12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F12" s="44"/>
       <c r="G12" s="42"/>
       <c r="H12" s="5"/>
     </row>
@@ -1068,18 +1000,14 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="41">
-        <v>23760055</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B14" s="41"/>
       <c r="C14" s="42"/>
       <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F14" s="41"/>
       <c r="G14" s="42"/>
       <c r="H14" s="5"/>
       <c r="K14" s="11"/>
@@ -1091,17 +1019,17 @@
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H16" s="12"/>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E17" s="6"/>
       <c r="H17" s="12"/>
@@ -1109,76 +1037,76 @@
     </row>
     <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H24" s="5"/>
     </row>
@@ -1188,42 +1116,42 @@
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H29" s="5"/>
     </row>
@@ -1233,62 +1161,62 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H36" s="5"/>
     </row>
@@ -1298,66 +1226,66 @@
     </row>
     <row r="38" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H44" s="5"/>
     </row>
@@ -1381,7 +1309,7 @@
     </row>
     <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1402,13 +1330,13 @@
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B65" s="33"/>
       <c r="C65" s="33"/>
@@ -1650,7 +1578,6 @@
 &amp;Z&amp;F&amp;C&amp;7 Retencion: 2 años
 &amp;R&amp;7 Relacionada con: 7.1-11 III</evenFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1674,7 +1601,7 @@
     <row r="1" spans="2:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -1686,26 +1613,26 @@
     </row>
     <row r="4" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -1713,23 +1640,23 @@
     <row r="6" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="14"/>
@@ -1737,36 +1664,36 @@
     <row r="8" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="14"/>
@@ -1774,20 +1701,20 @@
     <row r="11" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19"/>
       <c r="C11" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="14"/>
@@ -1795,10 +1722,10 @@
     <row r="13" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19"/>
       <c r="C13" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="14"/>
@@ -1806,10 +1733,10 @@
     <row r="14" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19"/>
       <c r="C14" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="14"/>
@@ -1817,17 +1744,17 @@
     <row r="15" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="14"/>
@@ -1835,10 +1762,10 @@
     <row r="17" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="14"/>
@@ -1846,10 +1773,10 @@
     <row r="18" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="14"/>
@@ -1857,10 +1784,10 @@
     <row r="19" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
       <c r="C19" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="14"/>
@@ -1868,10 +1795,10 @@
     <row r="20" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19"/>
       <c r="C20" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="14"/>
@@ -1879,29 +1806,29 @@
     <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
       <c r="C21" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E22" s="20"/>
     </row>
     <row r="23" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19"/>
       <c r="C23" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="14"/>
@@ -1909,10 +1836,10 @@
     <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="19"/>
       <c r="C24" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="14"/>
@@ -1920,20 +1847,20 @@
     <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="19"/>
       <c r="C25" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="14"/>
     </row>
     <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="14"/>
@@ -1941,7 +1868,7 @@
     <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="19"/>
       <c r="C27" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="14"/>
@@ -1949,10 +1876,10 @@
     <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="19"/>
       <c r="C28" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="14"/>
@@ -1960,10 +1887,10 @@
     <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="19"/>
       <c r="C29" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="14"/>
@@ -1971,10 +1898,10 @@
     <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19"/>
       <c r="C30" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="14"/>
@@ -1982,7 +1909,7 @@
     <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="19"/>
       <c r="C31" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="14"/>
@@ -1990,10 +1917,10 @@
     <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="19"/>
       <c r="C32" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="14"/>
@@ -2001,10 +1928,10 @@
     <row r="33" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="24"/>
       <c r="C33" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E33" s="26"/>
     </row>

</xml_diff>